<commit_message>
User Story ## 23 completed ## 30 minutes, The owner is now tied to all rental items
</commit_message>
<xml_diff>
--- a/Rubric-Sprint 3v1.xlsx
+++ b/Rubric-Sprint 3v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruce\Desktop\IS 413\chef-masterspr3\chef-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruce\Desktop\winter semester 2015\IS 413\chef-masterspr3\chef-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -110,6 +110,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
         <scheme val="major"/>
       </rPr>
       <t>employee</t>
@@ -119,6 +120,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
         <scheme val="major"/>
       </rPr>
       <t xml:space="preserve"> login credentials against Active Directory</t>
@@ -165,18 +167,21 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
@@ -184,6 +189,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
@@ -191,6 +197,7 @@
       <sz val="12"/>
       <color rgb="FF008000"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
@@ -204,6 +211,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="major"/>
     </font>
   </fonts>
@@ -999,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1101,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="2">
         <f>SUM(C8:C12)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(D8:D12)</f>
@@ -1106,7 +1114,9 @@
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
       <c r="D8" s="2">
         <v>10</v>
       </c>
@@ -1184,7 +1194,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="2">
         <f>SUM(C15:C16)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F14" s="2">
         <f>SUM(D15:D16)</f>
@@ -1212,7 +1222,9 @@
       <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2">
+        <v>10</v>
+      </c>
       <c r="D16" s="2">
         <v>10</v>
       </c>
@@ -1238,7 +1250,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="2">
         <f>SUM(C19:C23)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F18" s="2">
         <f>SUM(D19:D23)</f>
@@ -1264,7 +1276,9 @@
       <c r="B20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2">
+        <v>15</v>
+      </c>
       <c r="D20" s="2">
         <v>15</v>
       </c>
@@ -1329,7 +1343,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="2">
         <f>SUM(E7:E24)</f>
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F25" s="2">
         <f>SUM(F7:F24)</f>
@@ -1361,7 +1375,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="2">
         <f>E25*E26</f>
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F27" s="10">
         <f>F25*F26</f>
@@ -1379,7 +1393,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="11">
         <f>E27/F27</f>
-        <v>0.14814814814814814</v>
+        <v>0.40740740740740738</v>
       </c>
       <c r="G28" s="5"/>
     </row>

</xml_diff>

<commit_message>
User Story ## 23 Completed ## 20 minutes, It wasn't working properly because the transactions of a user are always on record so I had to get the rental Items that hadn't been returned yet
</commit_message>
<xml_diff>
--- a/Rubric-Sprint 3v1.xlsx
+++ b/Rubric-Sprint 3v1.xlsx
@@ -1008,7 +1008,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="2">
         <f>SUM(C8:C12)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(D8:D12)</f>
@@ -1129,7 +1129,9 @@
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
       <c r="D9" s="2">
         <v>5</v>
       </c>
@@ -1343,7 +1345,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="2">
         <f>SUM(E7:E24)</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F25" s="2">
         <f>SUM(F7:F24)</f>
@@ -1375,7 +1377,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="2">
         <f>E25*E26</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F27" s="10">
         <f>F25*F26</f>
@@ -1393,7 +1395,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="11">
         <f>E27/F27</f>
-        <v>0.40740740740740738</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G28" s="5"/>
     </row>

</xml_diff>

<commit_message>
user story ## 20 Completed ## 1 hour, an email is now able to be sent with a link for a user to reset their password
</commit_message>
<xml_diff>
--- a/Rubric-Sprint 3v1.xlsx
+++ b/Rubric-Sprint 3v1.xlsx
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1252,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="2">
         <f>SUM(C19:C23)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F18" s="2">
         <f>SUM(D19:D23)</f>
@@ -1319,7 +1319,9 @@
       <c r="B23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2">
+        <v>10</v>
+      </c>
       <c r="D23" s="2">
         <v>10</v>
       </c>
@@ -1345,7 +1347,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="2">
         <f>SUM(E7:E24)</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F25" s="2">
         <f>SUM(F7:F24)</f>
@@ -1377,7 +1379,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="2">
         <f>E25*E26</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F27" s="10">
         <f>F25*F26</f>
@@ -1395,7 +1397,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="11">
         <f>E27/F27</f>
-        <v>0.44444444444444442</v>
+        <v>0.51851851851851849</v>
       </c>
       <c r="G28" s="5"/>
     </row>

</xml_diff>

<commit_message>
user story ## 22 completed ## 2 hours, working on viewing overdue items, I am able to see the items that are 30, 60, 90+ days overdue, but I need to make it a batch process and format it a bit differently
</commit_message>
<xml_diff>
--- a/Rubric-Sprint 3v1.xlsx
+++ b/Rubric-Sprint 3v1.xlsx
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1252,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="2">
         <f>SUM(C19:C23)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F18" s="2">
         <f>SUM(D19:D23)</f>
@@ -1293,7 +1293,9 @@
       <c r="B21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2">
+        <v>15</v>
+      </c>
       <c r="D21" s="2">
         <v>15</v>
       </c>
@@ -1306,7 +1308,9 @@
       <c r="B22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2">
+        <v>10</v>
+      </c>
       <c r="D22" s="2">
         <v>15</v>
       </c>
@@ -1347,7 +1351,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="2">
         <f>SUM(E7:E24)</f>
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F25" s="2">
         <f>SUM(F7:F24)</f>
@@ -1379,7 +1383,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="2">
         <f>E25*E26</f>
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F27" s="10">
         <f>F25*F26</f>
@@ -1397,7 +1401,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="11">
         <f>E27/F27</f>
-        <v>0.51851851851851849</v>
+        <v>0.70370370370370372</v>
       </c>
       <c r="G28" s="5"/>
     </row>

</xml_diff>

<commit_message>
user story 29 completed 1 hour, working on getting users for certain transactions
</commit_message>
<xml_diff>
--- a/Rubric-Sprint 3v1.xlsx
+++ b/Rubric-Sprint 3v1.xlsx
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="2">
         <f>SUM(C8:C12)</f>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(D8:D12)</f>
@@ -1157,7 +1157,9 @@
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
       <c r="D11" s="2">
         <v>8</v>
       </c>
@@ -1351,7 +1353,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="2">
         <f>SUM(E7:E24)</f>
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F25" s="2">
         <f>SUM(F7:F24)</f>
@@ -1383,7 +1385,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="2">
         <f>E25*E26</f>
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F27" s="10">
         <f>F25*F26</f>
@@ -1401,7 +1403,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="11">
         <f>E27/F27</f>
-        <v>0.70370370370370372</v>
+        <v>0.76296296296296295</v>
       </c>
       <c r="G28" s="5"/>
     </row>

</xml_diff>

<commit_message>
User story ## 31 completed ## 2 hours, It isn't quite working, I am able to log in with some users but not with all of them
</commit_message>
<xml_diff>
--- a/Rubric-Sprint 3v1.xlsx
+++ b/Rubric-Sprint 3v1.xlsx
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1254,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="2">
         <f>SUM(C19:C23)</f>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F18" s="2">
         <f>SUM(D19:D23)</f>
@@ -1267,7 +1267,9 @@
       <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2">
+        <v>15</v>
+      </c>
       <c r="D19" s="2">
         <v>15</v>
       </c>
@@ -1311,7 +1313,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D22" s="2">
         <v>15</v>
@@ -1353,7 +1355,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="2">
         <f>SUM(E7:E24)</f>
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="F25" s="2">
         <f>SUM(F7:F24)</f>
@@ -1385,7 +1387,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="2">
         <f>E25*E26</f>
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="F27" s="10">
         <f>F25*F26</f>
@@ -1403,7 +1405,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="11">
         <f>E27/F27</f>
-        <v>0.76296296296296295</v>
+        <v>0.91111111111111109</v>
       </c>
       <c r="G28" s="5"/>
     </row>

</xml_diff>

<commit_message>
Refactoring of some code
</commit_message>
<xml_diff>
--- a/Rubric-Sprint 3v1.xlsx
+++ b/Rubric-Sprint 3v1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="2">
         <f>SUM(C8:C12)</f>
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(D8:D12)</f>
@@ -1144,7 +1144,9 @@
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
       <c r="D10" s="2">
         <v>5</v>
       </c>
@@ -1172,7 +1174,9 @@
       <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2">
+        <v>7</v>
+      </c>
       <c r="D12" s="2">
         <v>7</v>
       </c>
@@ -1355,7 +1359,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="2">
         <f>SUM(E7:E24)</f>
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F25" s="2">
         <f>SUM(F7:F24)</f>
@@ -1387,7 +1391,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="2">
         <f>E25*E26</f>
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F27" s="10">
         <f>F25*F26</f>
@@ -1405,7 +1409,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="11">
         <f>E27/F27</f>
-        <v>0.91111111111111109</v>
+        <v>1</v>
       </c>
       <c r="G28" s="5"/>
     </row>

</xml_diff>